<commit_message>
Add missing Total N
</commit_message>
<xml_diff>
--- a/Data/DWR_1981-2017_Surface main and qaqc.xlsx
+++ b/Data/DWR_1981-2017_Surface main and qaqc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="10056"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17496" windowHeight="10056" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DWRprimary" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="DWRfinal" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1490,7 +1489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10508,8 +10507,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F163" sqref="F163"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="J167" sqref="J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19263,6 +19264,9 @@
       <c r="L114" s="17">
         <v>0.02</v>
       </c>
+      <c r="M114" s="17">
+        <v>2.82</v>
+      </c>
       <c r="N114" s="17"/>
       <c r="O114" s="17">
         <v>67</v>
@@ -19337,6 +19341,9 @@
       <c r="L115" s="17">
         <v>0.11</v>
       </c>
+      <c r="M115" s="17">
+        <v>2.9099999999999997</v>
+      </c>
       <c r="N115" s="17"/>
       <c r="O115" s="17">
         <v>58</v>
@@ -19409,6 +19416,9 @@
       <c r="L116" s="17">
         <v>0.04</v>
       </c>
+      <c r="M116" s="17">
+        <v>3.14</v>
+      </c>
       <c r="N116" s="17"/>
       <c r="O116" s="17">
         <v>56</v>
@@ -19485,6 +19495,9 @@
       <c r="L117" s="17">
         <v>0.05</v>
       </c>
+      <c r="M117" s="17">
+        <v>3.15</v>
+      </c>
       <c r="N117" s="17"/>
       <c r="O117" s="17">
         <v>130</v>
@@ -19552,6 +19565,9 @@
       <c r="L118" s="17">
         <v>0.08</v>
       </c>
+      <c r="M118" s="17">
+        <v>3.18</v>
+      </c>
       <c r="N118" s="17"/>
       <c r="O118" s="17">
         <v>95</v>
@@ -19616,6 +19632,9 @@
       <c r="L119" s="17">
         <v>0.09</v>
       </c>
+      <c r="M119" s="17">
+        <v>4.99</v>
+      </c>
       <c r="N119" s="17"/>
       <c r="O119" s="17">
         <v>150</v>
@@ -19692,6 +19711,9 @@
       <c r="L120" s="17">
         <v>0.02</v>
       </c>
+      <c r="M120" s="17">
+        <v>2.52</v>
+      </c>
       <c r="N120" s="17"/>
       <c r="O120" s="17">
         <v>56</v>
@@ -19768,6 +19790,9 @@
       <c r="L121" s="17">
         <v>0.04</v>
       </c>
+      <c r="M121" s="17">
+        <v>3.04</v>
+      </c>
       <c r="N121" s="17"/>
       <c r="O121" s="17">
         <v>110</v>
@@ -19838,6 +19863,9 @@
       <c r="L122" s="17">
         <v>0.02</v>
       </c>
+      <c r="M122" s="17">
+        <v>2.82</v>
+      </c>
       <c r="N122" s="17"/>
       <c r="O122" s="17">
         <v>89</v>
@@ -19914,6 +19942,9 @@
       <c r="L123" s="17">
         <v>0.06</v>
       </c>
+      <c r="M123" s="17">
+        <v>3.2600000000000002</v>
+      </c>
       <c r="N123" s="17"/>
       <c r="O123" s="17">
         <v>95</v>
@@ -19984,6 +20015,9 @@
       <c r="L124" s="17">
         <v>0.02</v>
       </c>
+      <c r="M124" s="17">
+        <v>2.82</v>
+      </c>
       <c r="N124" s="17"/>
       <c r="O124" s="17">
         <v>89</v>
@@ -20060,6 +20094,9 @@
       <c r="L125" s="17">
         <v>0.02</v>
       </c>
+      <c r="M125" s="17">
+        <v>1.82</v>
+      </c>
       <c r="N125" s="17"/>
       <c r="O125" s="17">
         <v>70</v>
@@ -20136,6 +20173,9 @@
       <c r="L126" s="17">
         <v>0.02</v>
       </c>
+      <c r="M126" s="17">
+        <v>1.92</v>
+      </c>
       <c r="N126" s="17"/>
       <c r="O126" s="17">
         <v>32</v>
@@ -20209,6 +20249,9 @@
       <c r="L127" s="17">
         <v>0.09</v>
       </c>
+      <c r="M127" s="17">
+        <v>4.09</v>
+      </c>
       <c r="N127" s="17"/>
       <c r="O127" s="17">
         <v>150</v>
@@ -20285,6 +20328,9 @@
       <c r="L128" s="17">
         <v>0.02</v>
       </c>
+      <c r="M128" s="17">
+        <v>3.12</v>
+      </c>
       <c r="N128" s="17"/>
       <c r="O128" s="17">
         <v>74</v>
@@ -20361,6 +20407,9 @@
       <c r="L129" s="17">
         <v>0.04</v>
       </c>
+      <c r="M129" s="17">
+        <v>4.1399999999999997</v>
+      </c>
       <c r="N129" s="17"/>
       <c r="O129" s="17">
         <v>140</v>
@@ -20431,6 +20480,9 @@
       <c r="L130" s="17">
         <v>0.03</v>
       </c>
+      <c r="M130" s="17">
+        <v>2.5299999999999998</v>
+      </c>
       <c r="N130" s="17"/>
       <c r="O130" s="17">
         <v>94</v>
@@ -20507,6 +20559,9 @@
       <c r="L131" s="17">
         <v>0.04</v>
       </c>
+      <c r="M131" s="17">
+        <v>2.64</v>
+      </c>
       <c r="N131" s="17"/>
       <c r="O131" s="17">
         <v>67</v>
@@ -20577,6 +20632,9 @@
       <c r="L132" s="17">
         <v>0.03</v>
       </c>
+      <c r="M132" s="17">
+        <v>2.13</v>
+      </c>
       <c r="N132" s="17"/>
       <c r="O132" s="17">
         <v>60</v>
@@ -20651,6 +20709,9 @@
       <c r="L133" s="17">
         <v>0.02</v>
       </c>
+      <c r="M133" s="17">
+        <v>1.92</v>
+      </c>
       <c r="N133" s="17"/>
       <c r="O133" s="17">
         <v>55</v>
@@ -20727,6 +20788,9 @@
       <c r="L134" s="17">
         <v>0.02</v>
       </c>
+      <c r="M134" s="17">
+        <v>1.62</v>
+      </c>
       <c r="N134" s="17"/>
       <c r="O134" s="17">
         <v>38</v>
@@ -20801,7 +20865,9 @@
       <c r="L135" s="147">
         <v>0.03</v>
       </c>
-      <c r="M135" s="148"/>
+      <c r="M135" s="17">
+        <v>2.5299999999999998</v>
+      </c>
       <c r="N135" s="148"/>
       <c r="O135" s="147">
         <v>64</v>
@@ -20880,7 +20946,9 @@
       <c r="L136" s="147">
         <v>0.05</v>
       </c>
-      <c r="M136" s="148"/>
+      <c r="M136" s="17">
+        <v>3.55</v>
+      </c>
       <c r="N136" s="148"/>
       <c r="O136" s="147">
         <v>54</v>
@@ -20959,7 +21027,9 @@
       <c r="L137" s="147">
         <v>0.04</v>
       </c>
-      <c r="M137" s="148"/>
+      <c r="M137" s="17">
+        <v>4.24</v>
+      </c>
       <c r="N137" s="148"/>
       <c r="O137" s="147">
         <v>200</v>
@@ -21032,7 +21102,9 @@
       <c r="L138" s="147">
         <v>0.22</v>
       </c>
-      <c r="M138" s="148"/>
+      <c r="M138" s="17">
+        <v>4.72</v>
+      </c>
       <c r="N138" s="148"/>
       <c r="O138" s="147">
         <v>150</v>
@@ -21105,7 +21177,9 @@
       <c r="L139" s="147">
         <v>0.13</v>
       </c>
-      <c r="M139" s="147"/>
+      <c r="M139" s="17">
+        <v>3.73</v>
+      </c>
       <c r="N139" s="147"/>
       <c r="O139" s="147">
         <v>220</v>
@@ -21184,7 +21258,9 @@
       <c r="L140" s="147">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M140" s="147"/>
+      <c r="M140" s="17">
+        <v>4.67</v>
+      </c>
       <c r="N140" s="147"/>
       <c r="O140" s="147">
         <v>220</v>
@@ -21263,7 +21339,9 @@
       <c r="L141" s="147">
         <v>0.06</v>
       </c>
-      <c r="M141" s="147"/>
+      <c r="M141" s="17">
+        <v>4.8599999999999994</v>
+      </c>
       <c r="N141" s="147"/>
       <c r="O141" s="147">
         <v>110</v>
@@ -21340,7 +21418,9 @@
       <c r="L142" s="147">
         <v>0.04</v>
       </c>
-      <c r="M142" s="147"/>
+      <c r="M142" s="17">
+        <v>4.74</v>
+      </c>
       <c r="N142" s="147"/>
       <c r="O142" s="147">
         <v>180</v>
@@ -21419,7 +21499,9 @@
       <c r="L143" s="147">
         <v>0.02</v>
       </c>
-      <c r="M143" s="147"/>
+      <c r="M143" s="17">
+        <v>3.52</v>
+      </c>
       <c r="N143" s="147"/>
       <c r="O143" s="147">
         <v>180</v>
@@ -21498,7 +21580,9 @@
       <c r="L144" s="147">
         <v>0.02</v>
       </c>
-      <c r="M144" s="147"/>
+      <c r="M144" s="17">
+        <v>3.22</v>
+      </c>
       <c r="N144" s="147"/>
       <c r="O144" s="147">
         <v>190</v>
@@ -21577,7 +21661,9 @@
       <c r="L145" s="147">
         <v>0.02</v>
       </c>
-      <c r="M145" s="147"/>
+      <c r="M145" s="17">
+        <v>3.42</v>
+      </c>
       <c r="N145" s="147"/>
       <c r="O145" s="147">
         <v>140</v>
@@ -21656,7 +21742,9 @@
       <c r="L146" s="147">
         <v>0.02</v>
       </c>
-      <c r="M146" s="147"/>
+      <c r="M146" s="17">
+        <v>4.42</v>
+      </c>
       <c r="N146" s="147"/>
       <c r="O146" s="147">
         <v>210</v>
@@ -21733,7 +21821,9 @@
       <c r="L147" s="147">
         <v>0.02</v>
       </c>
-      <c r="M147" s="147"/>
+      <c r="M147" s="17">
+        <v>2.62</v>
+      </c>
       <c r="N147" s="147"/>
       <c r="O147" s="147">
         <v>78</v>
@@ -21812,7 +21902,9 @@
       <c r="L148" s="147">
         <v>0.02</v>
       </c>
-      <c r="M148" s="147"/>
+      <c r="M148" s="17">
+        <v>3.02</v>
+      </c>
       <c r="N148" s="147"/>
       <c r="O148" s="147">
         <v>91</v>
@@ -21891,7 +21983,9 @@
       <c r="L149" s="147">
         <v>0.02</v>
       </c>
-      <c r="M149" s="147"/>
+      <c r="M149" s="17">
+        <v>3.92</v>
+      </c>
       <c r="N149" s="147"/>
       <c r="O149" s="147">
         <v>160</v>
@@ -21970,7 +22064,9 @@
       <c r="L150" s="147">
         <v>0.06</v>
       </c>
-      <c r="M150" s="147"/>
+      <c r="M150" s="17">
+        <v>4.1599999999999993</v>
+      </c>
       <c r="N150" s="147"/>
       <c r="O150" s="147">
         <v>200</v>
@@ -22049,7 +22145,9 @@
       <c r="L151" s="147">
         <v>0.03</v>
       </c>
-      <c r="M151" s="147"/>
+      <c r="M151" s="17">
+        <v>3.13</v>
+      </c>
       <c r="N151" s="147"/>
       <c r="O151" s="147">
         <v>84</v>
@@ -22128,7 +22226,9 @@
       <c r="L152" s="147">
         <v>0.04</v>
       </c>
-      <c r="M152" s="147"/>
+      <c r="M152" s="17">
+        <v>3.44</v>
+      </c>
       <c r="N152" s="147"/>
       <c r="O152" s="147">
         <v>110</v>
@@ -22206,6 +22306,9 @@
       <c r="L153" s="17">
         <v>0.02</v>
       </c>
+      <c r="M153" s="17">
+        <v>2.3199999999999998</v>
+      </c>
       <c r="N153" s="17"/>
       <c r="O153" s="17">
         <v>32</v>
@@ -22281,6 +22384,9 @@
       </c>
       <c r="L154" s="17">
         <v>0.02</v>
+      </c>
+      <c r="M154" s="17">
+        <v>2.3199999999999998</v>
       </c>
       <c r="N154" s="17"/>
       <c r="O154" s="17">

</xml_diff>